<commit_message>
rebalance units a little
</commit_message>
<xml_diff>
--- a/Modding resources/Land combat/terrain.xlsx
+++ b/Modding resources/Land combat/terrain.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="42">
   <si>
     <t>militia</t>
   </si>
@@ -104,13 +104,49 @@
   </si>
   <si>
     <t>NEW</t>
+  </si>
+  <si>
+    <t>Reworked 2.0</t>
+  </si>
+  <si>
+    <t>Worst case</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Unfavorable</t>
+  </si>
+  <si>
+    <t>mediocre</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>favorable</t>
+  </si>
+  <si>
+    <t>ideal</t>
+  </si>
+  <si>
+    <t>excellent</t>
+  </si>
+  <si>
+    <t>atck</t>
+  </si>
+  <si>
+    <t>def</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +154,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +216,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -187,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -199,6 +253,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,16 +561,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F8:Z80"/>
+  <dimension ref="F8:Z116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="H115" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="8" width="10.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="6:26" x14ac:dyDescent="0.25">
@@ -1493,7 +1552,7 @@
         <v>-0.30000000000000004</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" ref="M37:M48" si="6">M11+$M$34</f>
+        <f t="shared" ref="M37:M47" si="6">M11+$M$34</f>
         <v>-0.4</v>
       </c>
       <c r="N37" s="2">
@@ -3019,6 +3078,880 @@
         <v>-0.05</v>
       </c>
       <c r="N80" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="84" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="R84" t="s">
+        <v>33</v>
+      </c>
+      <c r="S84" t="s">
+        <v>40</v>
+      </c>
+      <c r="T84" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="85" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="R85" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="S85">
+        <v>-0.6</v>
+      </c>
+      <c r="T85">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="86" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="R86" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S86">
+        <v>0.45</v>
+      </c>
+      <c r="T86">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="87" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>30</v>
+      </c>
+      <c r="R87" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S87">
+        <v>-0.3</v>
+      </c>
+      <c r="T87">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="88" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>13</v>
+      </c>
+      <c r="K88">
+        <v>-0.1</v>
+      </c>
+      <c r="L88">
+        <v>-0.1</v>
+      </c>
+      <c r="M88">
+        <v>-0.2</v>
+      </c>
+      <c r="N88">
+        <v>-0.2</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S88">
+        <v>-0.15</v>
+      </c>
+      <c r="T88">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="89" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" t="s">
+        <v>15</v>
+      </c>
+      <c r="I89" t="s">
+        <v>14</v>
+      </c>
+      <c r="J89" t="s">
+        <v>16</v>
+      </c>
+      <c r="K89" t="s">
+        <v>17</v>
+      </c>
+      <c r="L89" t="s">
+        <v>18</v>
+      </c>
+      <c r="M89" t="s">
+        <v>19</v>
+      </c>
+      <c r="N89" t="s">
+        <v>20</v>
+      </c>
+      <c r="R89" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S89">
+        <v>0</v>
+      </c>
+      <c r="T89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>0</v>
+      </c>
+      <c r="G90" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="H90" s="8">
+        <v>-0.45</v>
+      </c>
+      <c r="I90" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="J90" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="K90" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="L90" s="7">
+        <v>0</v>
+      </c>
+      <c r="M90" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="N90" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S90">
+        <v>0.15</v>
+      </c>
+      <c r="T90">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="91" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>1</v>
+      </c>
+      <c r="G91" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="H91" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="I91" s="7">
+        <v>0</v>
+      </c>
+      <c r="J91" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="K91" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="L91" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="M91" s="7">
+        <v>0</v>
+      </c>
+      <c r="N91" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="R91" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S91">
+        <v>0.25</v>
+      </c>
+      <c r="T91">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="92" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>2</v>
+      </c>
+      <c r="G92" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="H92" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="I92" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="J92" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="K92" s="7">
+        <v>0</v>
+      </c>
+      <c r="L92" s="7">
+        <v>0</v>
+      </c>
+      <c r="M92" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="N92" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="R92" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="S92">
+        <v>0.4</v>
+      </c>
+      <c r="T92">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="93" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>3</v>
+      </c>
+      <c r="G93" s="14">
+        <v>0</v>
+      </c>
+      <c r="H93" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J93" s="7">
+        <v>0</v>
+      </c>
+      <c r="K93" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="L93" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="M93" s="7">
+        <v>0</v>
+      </c>
+      <c r="N93" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="94" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>4</v>
+      </c>
+      <c r="G94" s="7">
+        <v>0</v>
+      </c>
+      <c r="H94" s="7">
+        <v>0</v>
+      </c>
+      <c r="I94" s="7">
+        <v>0</v>
+      </c>
+      <c r="J94" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="K94" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="L94" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="M94" s="13">
+        <v>-0.3</v>
+      </c>
+      <c r="N94" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I95" s="7">
+        <v>0</v>
+      </c>
+      <c r="J95" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="K95" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="L95" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="M95" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="N95" s="3">
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="96" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>6</v>
+      </c>
+      <c r="G96" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="H96" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="I96" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="J96" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="K96" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="L96" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="M96" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="N96" s="4">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="97" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>7</v>
+      </c>
+      <c r="G97" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="H97" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="I97" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="J97" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="K97" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="L97" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="M97" s="10">
+        <v>-0.6</v>
+      </c>
+      <c r="N97" s="10">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="98" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>8</v>
+      </c>
+      <c r="G98" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H98" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I98" s="7">
+        <v>0</v>
+      </c>
+      <c r="J98" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="K98" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="L98" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="M98" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="N98" s="5">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="99" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="H99" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="I99" s="7">
+        <v>0</v>
+      </c>
+      <c r="J99" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="K99" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L99" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="M99" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="N99" s="12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="100" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+      <c r="G100" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="H100" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="I100" s="7">
+        <v>0</v>
+      </c>
+      <c r="J100" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="K100" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="L100" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="M100" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="N100" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="101" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
+        <v>11</v>
+      </c>
+      <c r="G101" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="H101" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="I101" s="7">
+        <v>0</v>
+      </c>
+      <c r="J101" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K101" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="L101" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="M101" s="4">
+        <v>-0.25</v>
+      </c>
+      <c r="N101" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="103" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
+        <v>21</v>
+      </c>
+      <c r="K103">
+        <v>-0.1</v>
+      </c>
+      <c r="L103">
+        <v>-0.1</v>
+      </c>
+      <c r="M103" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="N103" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="104" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>12</v>
+      </c>
+      <c r="H104" t="s">
+        <v>15</v>
+      </c>
+      <c r="I104" t="s">
+        <v>14</v>
+      </c>
+      <c r="J104" t="s">
+        <v>16</v>
+      </c>
+      <c r="K104" t="s">
+        <v>17</v>
+      </c>
+      <c r="L104" t="s">
+        <v>18</v>
+      </c>
+      <c r="M104" t="s">
+        <v>19</v>
+      </c>
+      <c r="N104" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F105" t="s">
+        <v>0</v>
+      </c>
+      <c r="G105" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="H105" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="I105" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="J105" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="K105" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L105" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="M105" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="N105" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>1</v>
+      </c>
+      <c r="G106" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="H106" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="J106" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K106" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="L106" s="7">
+        <v>0</v>
+      </c>
+      <c r="M106" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="N106" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="107" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>2</v>
+      </c>
+      <c r="G107" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="H107" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="I107" s="7">
+        <v>0</v>
+      </c>
+      <c r="J107" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="K107" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L107" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="M107" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="N107" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="108" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
+        <v>3</v>
+      </c>
+      <c r="G108" s="7">
+        <v>0</v>
+      </c>
+      <c r="H108" s="7">
+        <v>0</v>
+      </c>
+      <c r="I108" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="J108" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="K108" s="7">
+        <v>0</v>
+      </c>
+      <c r="L108" s="7">
+        <v>0</v>
+      </c>
+      <c r="M108" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="N108" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="109" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>4</v>
+      </c>
+      <c r="G109" s="7">
+        <v>0</v>
+      </c>
+      <c r="H109" s="7">
+        <v>0</v>
+      </c>
+      <c r="I109" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="J109" s="7">
+        <v>0</v>
+      </c>
+      <c r="K109" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="L109" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="M109" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="N109" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="110" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>5</v>
+      </c>
+      <c r="G110" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I110" s="7">
+        <v>0</v>
+      </c>
+      <c r="J110" s="7">
+        <v>0</v>
+      </c>
+      <c r="K110" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="L110" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="M110" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="N110" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
+        <v>6</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H111" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I111" s="7">
+        <v>0</v>
+      </c>
+      <c r="J111" s="7">
+        <v>0</v>
+      </c>
+      <c r="K111" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="L111" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="M111" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="N111" s="3">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="112" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
+        <v>7</v>
+      </c>
+      <c r="G112" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I112" s="7">
+        <v>0</v>
+      </c>
+      <c r="J112" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K112" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="L112" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="M112" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="N112" s="5">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="113" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>8</v>
+      </c>
+      <c r="G113" s="7">
+        <v>0</v>
+      </c>
+      <c r="H113" s="7">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="J113" s="7">
+        <v>0</v>
+      </c>
+      <c r="K113" s="7">
+        <v>0</v>
+      </c>
+      <c r="L113" s="7">
+        <v>0</v>
+      </c>
+      <c r="M113" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="N113" s="4">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="114" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
+        <v>9</v>
+      </c>
+      <c r="G114" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="H114" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="I114" s="7">
+        <v>0</v>
+      </c>
+      <c r="J114" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="K114" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L114" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="M114" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="N114" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="115" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F115" t="s">
+        <v>10</v>
+      </c>
+      <c r="G115" s="7">
+        <v>0</v>
+      </c>
+      <c r="H115" s="7">
+        <v>0</v>
+      </c>
+      <c r="I115" s="7">
+        <v>0</v>
+      </c>
+      <c r="J115" s="7">
+        <v>0</v>
+      </c>
+      <c r="K115" s="7">
+        <v>0</v>
+      </c>
+      <c r="L115" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="M115" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="N115" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="116" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F116" t="s">
+        <v>11</v>
+      </c>
+      <c r="G116" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H116" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I116" s="7">
+        <v>0</v>
+      </c>
+      <c r="J116" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="K116" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="L116" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="M116" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="N116" s="1">
         <v>0.15</v>
       </c>
     </row>

</xml_diff>